<commit_message>
fix upload file example
</commit_message>
<xml_diff>
--- a/excel/customer.xlsx
+++ b/excel/customer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CV\mephar\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33F4407-9BAB-458D-B4ED-48C7C07C7E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A200781-2235-4BD4-B577-B795A648FD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{30862236-D2CC-4FB6-A217-4AD4040DAC5A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Họ tên</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>bba@gmail.com</t>
+  </si>
+  <si>
+    <t>Facebook</t>
   </si>
 </sst>
 </file>
@@ -510,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D5FC41-910B-4730-8B14-5443D25142A5}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,14 +524,14 @@
     <col min="2" max="2" width="11.109375" customWidth="1"/>
     <col min="3" max="3" width="12.44140625" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="14" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" customWidth="1"/>
-    <col min="16" max="16" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -547,41 +550,44 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -597,38 +603,38 @@
       <c r="F2" s="3">
         <v>37928</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>14</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="4">
         <v>104.194571</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="R2" s="4">
         <v>19.384166</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -641,10 +647,10 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix toa do khach hang (file excel)
</commit_message>
<xml_diff>
--- a/excel/customer.xlsx
+++ b/excel/customer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CV\mephar\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A200781-2235-4BD4-B577-B795A648FD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001466D6-FF30-4D30-8B64-90A8F8EE3633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{30862236-D2CC-4FB6-A217-4AD4040DAC5A}"/>
   </bookViews>
@@ -104,28 +104,28 @@
     <t>Trạng thái</t>
   </si>
   <si>
-    <t>Kinh độ</t>
-  </si>
-  <si>
-    <t>Vĩ độ</t>
-  </si>
-  <si>
-    <t>0962547000</t>
-  </si>
-  <si>
     <t>a123</t>
   </si>
   <si>
     <t>b123</t>
   </si>
   <si>
-    <t>0962547001</t>
-  </si>
-  <si>
     <t>bba@gmail.com</t>
   </si>
   <si>
     <t>Facebook</t>
+  </si>
+  <si>
+    <t>Tọa độ</t>
+  </si>
+  <si>
+    <t>21.079350776626914, 105.80247286566104</t>
+  </si>
+  <si>
+    <t>0962447000</t>
+  </si>
+  <si>
+    <t>0912547001</t>
   </si>
 </sst>
 </file>
@@ -170,14 +170,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -513,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D5FC41-910B-4730-8B14-5443D25142A5}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,10 +525,10 @@
     <col min="9" max="9" width="15.5546875" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" customWidth="1"/>
     <col min="15" max="15" width="16.109375" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +548,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -581,18 +578,15 @@
         <v>21</v>
       </c>
       <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="R1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>20</v>
@@ -627,22 +621,19 @@
       <c r="P2">
         <v>1</v>
       </c>
-      <c r="Q2" s="4">
-        <v>104.194571</v>
-      </c>
-      <c r="R2" s="4">
-        <v>19.384166</v>
+      <c r="Q2" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E3">
         <v>0</v>

</xml_diff>